<commit_message>
updating for removal of compartment attribute from wc_lang.Submodel
</commit_message>
<xml_diff>
--- a/examples/transcription_translation_hybrid_model/model.xlsx
+++ b/examples/transcription_translation_hybrid_model/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -40,40 +40,56 @@
     <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="true" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$H$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$H$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Submodels!$A$1:$H$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Observables!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Observables!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Observables!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -85,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="109">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -147,190 +163,190 @@
     <t xml:space="preserve">Algorithm</t>
   </si>
   <si>
+    <t xml:space="preserve">Biomass reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objective function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdl_transcription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transcription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdl_translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdl_rna_degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNA degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdl_prot_degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">protein degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cytosol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empirical formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molecular weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNA (MPN001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUGAAAGUUUUGAUUAAUAAGAAUGAGUUGAACAAAAUCCUCAAAAAACUCAACAAUGUAAUCGUAUCUAACAAUAAGAUGAAACCAUACCACUCUUAUUUAUUAAUAGAGGCUACAGAAAAGGAAAUUAACUUCUAUGCUAACAACGAGUACUUUUCUGCUAAAUGUACCUUAGCCGAAAACAUUGAUGUACUUGAAGAAGGUGAAGUAAUUGUUAAAGGCAAAAUCUUUAGCGAACUCAUUAACGGAAUUAAAGAAGACAUCAUUACUAUUCAAGAGAAAGAUCAAACUCUUUUAGUCAAAACAAAAAAAACAAACAUUAACCUUAACACGAUUGAUAAGAAAGAAUUCCCCAGAAUCCGUUUCAACCAAAACGUUGAUUUGAAGGAAUUUGAUGAACUUAAAAUCCAACACAGCCUUUUAACUAAAGGACUUAAAAAGAUUGCCCAUGCUGUUUCUACAUUUAGAGAAUCCACUAGAAAAUUCAACGGGGUUAACUUCAACGGUUCCAAUGGUAAACAAAUCUUUUUAGAGGCAUCGGAUUCUUAUAAGCUCUCUGUUUAUGAAAUCAAACAAAAAACCGAUCCAUUUAAUUUCAUUGUCGAAACUAAUCUUUUGAGCUUCAUCAAUUCUUUUAACCCUGAAGGUGGUGAUUUAAUCAGUAUCUUCUUCCGCAAAGAACACAAGGAUGAUUUAAGUACCGAAUUACUGAUUAAGUUAGAUAACUUCUUAAUUAACUACACCUCAAUUAACGAAAGCUUUCCGCGGGUAAUGCAGUUGUUUGACUUUGAACCAGAAACCAAAGUAACCAUUCAAAAAAACGAACUUAAAGAUGCAUUACAAAGAAUCUUGACGUUAGCUCAAAACGAGCGCUUCUUUCUCUGUGACAUGCAAGUAACCAACUCCCACCUCAAAAUUAAUUCCAACGUUCAAAACAUUGGUGCAUCCUUAGAAGAAGUUACUUGCCUUAAGUUCGAAGGUCACAAACUCAACAUCGCUGUUAAUGCGCUUUCCCUCUUGGAACACAUUGACUCAUUUGAUACUGAUGAAAUUGAGCUUUACUUCCAGGGCAGUAACAAAUACUUUUUAAUUAGUUCGAACAACGAACCUGAACUUAAAGAAAUCCUAGUUCCUUCCAAGUAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10932H12244O6763N4389P1143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">protein (MPN001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MKVLINKNELNKILKKLNNVIVSNNKMKPYHSYLLIEATEKEINFYANNEYFSAKCTLAENIDVLEEGEVIVKGKIFSELINGIKEDIITIQEKDQTLLVKTKKTNINLNTIDKKEFPRIRFNQNVDLKEFDELKIQHSLLTKGLKKIAHAVSTFRESTRKFNGVNFNGSNGKQIFLEASDSYKLSVYEIKQKTDPFNFIVETNLLSFINSFNPEGGDLISIFFRKEHKDDLSTELLIKLDNFLINYTSINESFPRVMQLFDFEPETKVTIQKNELKDALQRILTLAQNERFFLCDMQVTNSHLKINSNVQNIGASLEEVTCLKFEGHKLNIAVNALSLLEHIDSFDTDEIELYFQGSNKYFLISSNNEPELKEILVPSK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1980H3146N237O596S7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pseudo_species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">molecules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prot[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submodel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reversible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">==&gt; rna[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">==&gt; prot[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna_degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna[c] ==&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prot_degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prot[c] ==&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat * (rna[c] / (k_m + rna[c]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat * rna[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat * prot[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coefficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Compartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biomass reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Objective function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mdl_transcription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transcription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mdl_translation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">translation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mdl_rna_degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNA degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mdl_prot_degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">protein degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cytosol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empirical formula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Molecular weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNA (MPN001)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUGAAAGUUUUGAUUAAUAAGAAUGAGUUGAACAAAAUCCUCAAAAAACUCAACAAUGUAAUCGUAUCUAACAAUAAGAUGAAACCAUACCACUCUUAUUUAUUAAUAGAGGCUACAGAAAAGGAAAUUAACUUCUAUGCUAACAACGAGUACUUUUCUGCUAAAUGUACCUUAGCCGAAAACAUUGAUGUACUUGAAGAAGGUGAAGUAAUUGUUAAAGGCAAAAUCUUUAGCGAACUCAUUAACGGAAUUAAAGAAGACAUCAUUACUAUUCAAGAGAAAGAUCAAACUCUUUUAGUCAAAACAAAAAAAACAAACAUUAACCUUAACACGAUUGAUAAGAAAGAAUUCCCCAGAAUCCGUUUCAACCAAAACGUUGAUUUGAAGGAAUUUGAUGAACUUAAAAUCCAACACAGCCUUUUAACUAAAGGACUUAAAAAGAUUGCCCAUGCUGUUUCUACAUUUAGAGAAUCCACUAGAAAAUUCAACGGGGUUAACUUCAACGGUUCCAAUGGUAAACAAAUCUUUUUAGAGGCAUCGGAUUCUUAUAAGCUCUCUGUUUAUGAAAUCAAACAAAAAACCGAUCCAUUUAAUUUCAUUGUCGAAACUAAUCUUUUGAGCUUCAUCAAUUCUUUUAACCCUGAAGGUGGUGAUUUAAUCAGUAUCUUCUUCCGCAAAGAACACAAGGAUGAUUUAAGUACCGAAUUACUGAUUAAGUUAGAUAACUUCUUAAUUAACUACACCUCAAUUAACGAAAGCUUUCCGCGGGUAAUGCAGUUGUUUGACUUUGAACCAGAAACCAAAGUAACCAUUCAAAAAAACGAACUUAAAGAUGCAUUACAAAGAAUCUUGACGUUAGCUCAAAACGAGCGCUUCUUUCUCUGUGACAUGCAAGUAACCAACUCCCACCUCAAAAUUAAUUCCAACGUUCAAAACAUUGGUGCAUCCUUAGAAGAAGUUACUUGCCUUAAGUUCGAAGGUCACAAACUCAACAUCGCUGUUAAUGCGCUUUCCCUCUUGGAACACAUUGACUCAUUUGAUACUGAUGAAAUUGAGCUUUACUUCCAGGGCAGUAACAAAUACUUUUUAAUUAGUUCGAACAACGAACCUGAACUUAAAGAAAUCCUAGUUCCUUCCAAGUAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C10932H12244O6763N4389P1143</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">protein (MPN001)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MKVLINKNELNKILKKLNNVIVSNNKMKPYHSYLLIEATEKEINFYANNEYFSAKCTLAENIDVLEEGEVIVKGKIFSELINGIKEDIITIQEKDQTLLVKTKKTNINLNTIDKKEFPRIRFNQNVDLKEFDELKIQHSLLTKGLKKIAHAVSTFRESTRKFNGVNFNGSNGKQIFLEASDSYKLSVYEIKQKTDPFNFIVETNLLSFINSFNPEGGDLISIFFRKEHKDDLSTELLIKLDNFLINYTSINESFPRVMQLFDFEPETKVTIQKNELKDALQRILTLAQNERFFLCDMQVTNSHLKINSNVQNIGASLEEVTCLKFEGHKLNIAVNALSLLEHIDSFDTDEIELYFQGSNKYFLISSNNEPELKEILVPSK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1980H3146N237O596S7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">protein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pseudo_species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rna[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prot[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cell[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submodel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reversible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">==&gt; rna[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">==&gt; prot[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rna_degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rna[c] ==&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prot_degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prot[c] ==&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat * (rna[c] / (k_m + rna[c]))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat * rna[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat * prot[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species type</t>
   </si>
   <si>
     <t xml:space="preserve">Model</t>
@@ -690,7 +706,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -776,7 +792,7 @@
   </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -786,27 +802,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>13</v>
@@ -817,13 +833,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0.00770163533955495</v>
@@ -831,13 +847,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.0320901472481456</v>
@@ -848,13 +864,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>155370.480849579</v>
@@ -862,13 +878,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>431.58466902661</v>
@@ -917,13 +933,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>13</v>
@@ -973,7 +989,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1012,9 +1028,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1538461538462"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1032,10 +1048,10 @@
         <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
@@ -1119,7 +1135,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1178,7 +1194,7 @@
         <v>93</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>94</v>
@@ -1241,7 +1257,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.63967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.74898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1262,16 +1278,16 @@
         <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>106</v>
@@ -1377,20 +1393,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1411,61 +1427,58 @@
         <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="C5" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1"/>
+  <autoFilter ref="A1:G1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1505,7 +1518,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1516,10 +1529,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>6.7E-017</v>
@@ -1557,9 +1570,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3765182186235"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4736842105263"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1571,19 +1584,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>13</v>
@@ -1594,56 +1607,56 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>348724.1</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>47</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>40031.7</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>30712200000</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1715,13 +1728,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1732,35 +1745,35 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1500</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1804,7 +1817,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1851,7 +1864,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1887,10 +1900,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1052631578947"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -1903,19 +1916,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>13</v>
@@ -1926,16 +1939,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>0</v>
@@ -1943,16 +1956,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" s="6" t="n">
         <v>0</v>
@@ -1960,16 +1973,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="E4" s="6" t="n">
         <v>0</v>
@@ -1977,16 +1990,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="E5" s="6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
updating for new Species table in wc_lang (Species definied explicitly rather than inline); changing wc_lang.core --> wc_lang
</commit_message>
<xml_diff>
--- a/examples/transcription_translation_hybrid_model/model.xlsx
+++ b/examples/transcription_translation_hybrid_model/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,83 +13,100 @@
     <sheet name="Submodels" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Compartments" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Species types" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Concentrations" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Observables" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Functions" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Reactions" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Rate laws" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Biomass components" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Biomass reactions" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Parameters" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Stop conditions" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="References" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Database references" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Species" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Concentrations" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Observables" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Functions" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Reactions" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Rate laws" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Biomass components" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Biomass reactions" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Parameters" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Stop conditions" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="References" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Database references" sheetId="17" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Functions!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Model!$A$1:$B$8</definedName>
-    <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Observables!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$Q$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Observables!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Observables!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Observables!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Observables!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Functions!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$Q$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Observables!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">Observables!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Observables!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Observables!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Functions!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$Q$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -101,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="109">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -253,6 +270,21 @@
     <t xml:space="preserve">pseudo_species</t>
   </si>
   <si>
+    <t xml:space="preserve">Species type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prot[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell[c]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Species</t>
   </si>
   <si>
@@ -262,18 +294,9 @@
     <t xml:space="preserve">Units</t>
   </si>
   <si>
-    <t xml:space="preserve">rna[c]</t>
-  </si>
-  <si>
     <t xml:space="preserve">molecules</t>
   </si>
   <si>
-    <t xml:space="preserve">prot[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cell[c]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Expression</t>
   </si>
   <si>
@@ -341,12 +364,6 @@
   </si>
   <si>
     <t xml:space="preserve">Coefficient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compartment</t>
   </si>
   <si>
     <t xml:space="preserve">Model</t>
@@ -440,7 +457,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -468,6 +485,14 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -519,7 +544,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -534,6 +559,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -706,7 +735,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -790,6 +819,141 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:I1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -797,32 +961,32 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>13</v>
@@ -836,10 +1000,10 @@
         <v>23</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0.00770163533955495</v>
@@ -850,10 +1014,10 @@
         <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.0320901472481456</v>
@@ -864,13 +1028,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>155370.480849579</v>
@@ -878,13 +1042,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>431.58466902661</v>
@@ -905,7 +1069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -936,10 +1100,10 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>13</v>
@@ -961,7 +1125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -969,9 +1133,9 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -989,7 +1153,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1011,7 +1175,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1030,7 +1194,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1048,10 +1212,10 @@
         <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
@@ -1107,7 +1271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1135,7 +1299,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1154,7 +1318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1240,7 +1404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1257,7 +1421,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1278,16 +1442,16 @@
         <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>106</v>
@@ -1297,7 +1461,7 @@
       <c r="A2" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="8" t="n">
         <v>272634</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -1395,7 +1559,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1405,8 +1569,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1572,7 +1736,7 @@
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1711,6 +1875,91 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H11" activeCellId="0" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1718,7 +1967,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1728,13 +1977,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1745,86 +1994,39 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1500</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:D1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1864,7 +2066,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1888,24 +2090,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1915,98 +2112,15 @@
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>58</v>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
+  <autoFilter ref="A1:D1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
revising Excel files for revisions to wc-lang
</commit_message>
<xml_diff>
--- a/examples/transcription_translation_hybrid_model/model.xlsx
+++ b/examples/transcription_translation_hybrid_model/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,16 +19,16 @@
     <sheet name="Functions" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Reactions" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Rate laws" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Biomass components" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Biomass reactions" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Biomass reactions" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Biomass components" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="Parameters" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Stop conditions" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="References" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="Database references" sheetId="17" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
     <definedName function="false" hidden="true" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
@@ -41,72 +41,88 @@
     <definedName function="false" hidden="true" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$F$1</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Submodels!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Submodels!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Submodels!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Submodels!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Submodels!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Concentrations!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Observables!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">Observables!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Observables!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Observables!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Observables!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -118,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="109">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -180,187 +196,187 @@
     <t xml:space="preserve">Algorithm</t>
   </si>
   <si>
+    <t xml:space="preserve">Objective function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdl_transcription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transcription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdl_translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdl_rna_degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNA degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdl_prot_degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">protein degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cytosol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empirical formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molecular weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNA (MPN001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUGAAAGUUUUGAUUAAUAAGAAUGAGUUGAACAAAAUCCUCAAAAAACUCAACAAUGUAAUCGUAUCUAACAAUAAGAUGAAACCAUACCACUCUUAUUUAUUAAUAGAGGCUACAGAAAAGGAAAUUAACUUCUAUGCUAACAACGAGUACUUUUCUGCUAAAUGUACCUUAGCCGAAAACAUUGAUGUACUUGAAGAAGGUGAAGUAAUUGUUAAAGGCAAAAUCUUUAGCGAACUCAUUAACGGAAUUAAAGAAGACAUCAUUACUAUUCAAGAGAAAGAUCAAACUCUUUUAGUCAAAACAAAAAAAACAAACAUUAACCUUAACACGAUUGAUAAGAAAGAAUUCCCCAGAAUCCGUUUCAACCAAAACGUUGAUUUGAAGGAAUUUGAUGAACUUAAAAUCCAACACAGCCUUUUAACUAAAGGACUUAAAAAGAUUGCCCAUGCUGUUUCUACAUUUAGAGAAUCCACUAGAAAAUUCAACGGGGUUAACUUCAACGGUUCCAAUGGUAAACAAAUCUUUUUAGAGGCAUCGGAUUCUUAUAAGCUCUCUGUUUAUGAAAUCAAACAAAAAACCGAUCCAUUUAAUUUCAUUGUCGAAACUAAUCUUUUGAGCUUCAUCAAUUCUUUUAACCCUGAAGGUGGUGAUUUAAUCAGUAUCUUCUUCCGCAAAGAACACAAGGAUGAUUUAAGUACCGAAUUACUGAUUAAGUUAGAUAACUUCUUAAUUAACUACACCUCAAUUAACGAAAGCUUUCCGCGGGUAAUGCAGUUGUUUGACUUUGAACCAGAAACCAAAGUAACCAUUCAAAAAAACGAACUUAAAGAUGCAUUACAAAGAAUCUUGACGUUAGCUCAAAACGAGCGCUUCUUUCUCUGUGACAUGCAAGUAACCAACUCCCACCUCAAAAUUAAUUCCAACGUUCAAAACAUUGGUGCAUCCUUAGAAGAAGUUACUUGCCUUAAGUUCGAAGGUCACAAACUCAACAUCGCUGUUAAUGCGCUUUCCCUCUUGGAACACAUUGACUCAUUUGAUACUGAUGAAAUUGAGCUUUACUUCCAGGGCAGUAACAAAUACUUUUUAAUUAGUUCGAACAACGAACCUGAACUUAAAGAAAUCCUAGUUCCUUCCAAGUAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10932H12244O6763N4389P1143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">protein (MPN001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MKVLINKNELNKILKKLNNVIVSNNKMKPYHSYLLIEATEKEINFYANNEYFSAKCTLAENIDVLEEGEVIVKGKIFSELINGIKEDIITIQEKDQTLLVKTKKTNINLNTIDKKEFPRIRFNQNVDLKEFDELKIQHSLLTKGLKKIAHAVSTFRESTRKFNGVNFNGSNGKQIFLEASDSYKLSVYEIKQKTDPFNFIVETNLLSFINSFNPEGGDLISIFFRKEHKDDLSTELLIKLDNFLINYTSINESFPRVMQLFDFEPETKVTIQKNELKDALQRILTLAQNERFFLCDMQVTNSHLKINSNVQNIGASLEEVTCLKFEGHKLNIAVNALSLLEHIDSFDTDEIELYFQGSNKYFLISSNNEPELKEILVPSK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1980H3146N237O596S7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pseudo_species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prot[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">molecules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submodel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reversible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">==&gt; rna[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">==&gt; prot[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna_degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna[c] ==&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prot_degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prot[c] ==&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat * (rna[c] / (k_m + rna[c]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat * rna[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat * prot[c]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Biomass reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Objective function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mdl_transcription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transcription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mdl_translation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">translation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mdl_rna_degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNA degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mdl_prot_degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">protein degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cytosol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empirical formula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Molecular weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNA (MPN001)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUGAAAGUUUUGAUUAAUAAGAAUGAGUUGAACAAAAUCCUCAAAAAACUCAACAAUGUAAUCGUAUCUAACAAUAAGAUGAAACCAUACCACUCUUAUUUAUUAAUAGAGGCUACAGAAAAGGAAAUUAACUUCUAUGCUAACAACGAGUACUUUUCUGCUAAAUGUACCUUAGCCGAAAACAUUGAUGUACUUGAAGAAGGUGAAGUAAUUGUUAAAGGCAAAAUCUUUAGCGAACUCAUUAACGGAAUUAAAGAAGACAUCAUUACUAUUCAAGAGAAAGAUCAAACUCUUUUAGUCAAAACAAAAAAAACAAACAUUAACCUUAACACGAUUGAUAAGAAAGAAUUCCCCAGAAUCCGUUUCAACCAAAACGUUGAUUUGAAGGAAUUUGAUGAACUUAAAAUCCAACACAGCCUUUUAACUAAAGGACUUAAAAAGAUUGCCCAUGCUGUUUCUACAUUUAGAGAAUCCACUAGAAAAUUCAACGGGGUUAACUUCAACGGUUCCAAUGGUAAACAAAUCUUUUUAGAGGCAUCGGAUUCUUAUAAGCUCUCUGUUUAUGAAAUCAAACAAAAAACCGAUCCAUUUAAUUUCAUUGUCGAAACUAAUCUUUUGAGCUUCAUCAAUUCUUUUAACCCUGAAGGUGGUGAUUUAAUCAGUAUCUUCUUCCGCAAAGAACACAAGGAUGAUUUAAGUACCGAAUUACUGAUUAAGUUAGAUAACUUCUUAAUUAACUACACCUCAAUUAACGAAAGCUUUCCGCGGGUAAUGCAGUUGUUUGACUUUGAACCAGAAACCAAAGUAACCAUUCAAAAAAACGAACUUAAAGAUGCAUUACAAAGAAUCUUGACGUUAGCUCAAAACGAGCGCUUCUUUCUCUGUGACAUGCAAGUAACCAACUCCCACCUCAAAAUUAAUUCCAACGUUCAAAACAUUGGUGCAUCCUUAGAAGAAGUUACUUGCCUUAAGUUCGAAGGUCACAAACUCAACAUCGCUGUUAAUGCGCUUUCCCUCUUGGAACACAUUGACUCAUUUGAUACUGAUGAAAUUGAGCUUUACUUCCAGGGCAGUAACAAAUACUUUUUAAUUAGUUCGAACAACGAACCUGAACUUAAAGAAAUCCUAGUUCCUUCCAAGUAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C10932H12244O6763N4389P1143</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">protein (MPN001)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MKVLINKNELNKILKKLNNVIVSNNKMKPYHSYLLIEATEKEINFYANNEYFSAKCTLAENIDVLEEGEVIVKGKIFSELINGIKEDIITIQEKDQTLLVKTKKTNINLNTIDKKEFPRIRFNQNVDLKEFDELKIQHSLLTKGLKKIAHAVSTFRESTRKFNGVNFNGSNGKQIFLEASDSYKLSVYEIKQKTDPFNFIVETNLLSFINSFNPEGGDLISIFFRKEHKDDLSTELLIKLDNFLINYTSINESFPRVMQLFDFEPETKVTIQKNELKDALQRILTLAQNERFFLCDMQVTNSHLKINSNVQNIGASLEEVTCLKFEGHKLNIAVNALSLLEHIDSFDTDEIELYFQGSNKYFLISSNNEPELKEILVPSK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1980H3146N237O596S7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">protein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pseudo_species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rna[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prot[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cell[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submodel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reversible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">==&gt; rna[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">==&gt; prot[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rna_degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rna[c] ==&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prot_degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prot[c] ==&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat * (rna[c] / (k_m + rna[c]))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat * rna[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat * prot[c]</t>
   </si>
   <si>
     <t xml:space="preserve">Coefficient</t>
@@ -735,7 +751,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -831,10 +847,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -847,19 +863,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>13</v>
@@ -870,16 +886,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="7" t="n">
         <v>0</v>
@@ -887,16 +903,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="7" t="n">
         <v>0</v>
@@ -904,16 +920,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>68</v>
       </c>
       <c r="E4" s="7" t="n">
         <v>0</v>
@@ -921,16 +937,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>70</v>
       </c>
       <c r="E5" s="7" t="n">
         <v>0</v>
@@ -966,27 +982,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>13</v>
@@ -997,13 +1013,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>77</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0.00770163533955495</v>
@@ -1011,13 +1027,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.0320901472481456</v>
@@ -1028,13 +1044,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>155370.480849579</v>
@@ -1042,13 +1058,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>431.58466902661</v>
@@ -1074,14 +1090,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1097,23 +1113,17 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1"/>
+  <autoFilter ref="A1:E1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1130,14 +1140,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1153,17 +1163,23 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
+  <autoFilter ref="A1:G1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1194,7 +1210,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1212,10 +1228,10 @@
         <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
@@ -1299,7 +1315,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1358,7 +1374,7 @@
         <v>93</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>94</v>
@@ -1421,7 +1437,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1442,16 +1458,16 @@
         <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>106</v>
@@ -1557,20 +1573,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1588,61 +1604,58 @@
         <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>28</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1"/>
+  <autoFilter ref="A1:F1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1682,7 +1695,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1693,10 +1706,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>33</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>6.7E-017</v>
@@ -1736,7 +1749,7 @@
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1748,19 +1761,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>13</v>
@@ -1771,56 +1784,56 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>348724.1</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>46</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>40031.7</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>30712200000</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1877,7 +1890,7 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1887,8 +1900,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1899,10 +1912,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>13</v>
@@ -1913,35 +1926,35 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1977,13 +1990,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1994,35 +2007,35 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1500</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2066,7 +2079,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -2113,7 +2126,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
add model with comprehensive tests for dynamic expressions; migrate other models to new version obj-tables
</commit_message>
<xml_diff>
--- a/examples/transcription_translation_hybrid_model/model.xlsx
+++ b/examples/transcription_translation_hybrid_model/model.xlsx
@@ -7,30 +7,30 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="993" visibility="visible" windowHeight="13965" windowWidth="28695"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!_Table of contents" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Model" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Taxon" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Environment" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Submodels" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Compartments" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Species types" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Species" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Initial species concentrations" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Observables" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Functions" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Reactions" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Rate laws" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!dFBA objectives" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!dFBA objective reactions" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!dFBA objective species" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Parameters" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Stop conditions" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Observations" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Observation sets" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Conclusions" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!References" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Authors" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!Changes" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!_Table of contents" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Model" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Taxon" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Environment" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Submodels" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Compartments" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Species types" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Species" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Initial species concentrations" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Observables" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Functions" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Reactions" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Rate laws" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!dFBA objectives" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!dFBA objective reactions" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!dFBA objective species" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Parameters" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Stop conditions" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Observations" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Observation sets" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Conclusions" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!References" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Authors" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Changes" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
   <definedNames>
     <definedName localSheetId="1" name="_FilterDatabase_0">Model!$A$1:$B$7</definedName>
@@ -93,22 +93,22 @@
     <definedName localSheetId="21" name="_FilterDatabase_0_0">References!$A$1:$Q$1</definedName>
     <definedName localSheetId="21" name="_FilterDatabase_0_0_0">References!$A$1:$Q$1</definedName>
     <definedName localSheetId="21" name="_FilterDatabase_0_0_0_0">References!$A$1:$Q$1</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'!_Table of contents'!$A$1:$C$24</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'!Model'!$A$1:$B$12</definedName>
-    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'!Taxon'!$A$1:$A$6</definedName>
-    <definedName hidden="1" localSheetId="4" name="_xlnm._FilterDatabase">'!Submodels'!$A$1:$G$5</definedName>
-    <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">'!Compartments'!$A$2:$H$3</definedName>
-    <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">'!Species types'!$A$2:$K$5</definedName>
-    <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">'!Initial species concentrations'!$A$1:$E$4</definedName>
-    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">'!Observables'!$A$1:$D$1</definedName>
-    <definedName hidden="1" localSheetId="10" name="_xlnm._FilterDatabase">'!Functions'!$A$1:$D$2</definedName>
-    <definedName hidden="1" localSheetId="11" name="_xlnm._FilterDatabase">'!Reactions'!$A$2:$J$6</definedName>
-    <definedName hidden="1" localSheetId="12" name="_xlnm._FilterDatabase">'!Rate laws'!$A$1:$G$5</definedName>
-    <definedName hidden="1" localSheetId="14" name="_xlnm._FilterDatabase">'!dFBA objective reactions'!$A$1:$E$1</definedName>
-    <definedName hidden="1" localSheetId="15" name="_xlnm._FilterDatabase">'!dFBA objective species'!$A$1:$G$1</definedName>
-    <definedName hidden="1" localSheetId="16" name="_xlnm._FilterDatabase">'!Parameters'!$A$1:$H$10</definedName>
-    <definedName hidden="1" localSheetId="17" name="_xlnm._FilterDatabase">'!Stop conditions'!$A$1:$D$1</definedName>
-    <definedName hidden="1" localSheetId="21" name="_xlnm._FilterDatabase">'!References'!$A$1:$Q$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'!!_Table of contents'!$A$1:$C$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'!!Model'!$A$1:$B$12</definedName>
+    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'!!Taxon'!$A$1:$A$6</definedName>
+    <definedName hidden="1" localSheetId="4" name="_xlnm._FilterDatabase">'!!Submodels'!$A$1:$G$5</definedName>
+    <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">'!!Compartments'!$A$2:$H$3</definedName>
+    <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">'!!Species types'!$A$2:$K$5</definedName>
+    <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">'!!Initial species concentrations'!$A$1:$E$4</definedName>
+    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">'!!Observables'!$A$1:$D$1</definedName>
+    <definedName hidden="1" localSheetId="10" name="_xlnm._FilterDatabase">'!!Functions'!$A$1:$D$2</definedName>
+    <definedName hidden="1" localSheetId="11" name="_xlnm._FilterDatabase">'!!Reactions'!$A$2:$J$6</definedName>
+    <definedName hidden="1" localSheetId="12" name="_xlnm._FilterDatabase">'!!Rate laws'!$A$1:$G$5</definedName>
+    <definedName hidden="1" localSheetId="14" name="_xlnm._FilterDatabase">'!!dFBA objective reactions'!$A$1:$E$1</definedName>
+    <definedName hidden="1" localSheetId="15" name="_xlnm._FilterDatabase">'!!dFBA objective species'!$A$1:$G$1</definedName>
+    <definedName hidden="1" localSheetId="16" name="_xlnm._FilterDatabase">'!!Parameters'!$A$1:$H$10</definedName>
+    <definedName hidden="1" localSheetId="17" name="_xlnm._FilterDatabase">'!!Stop conditions'!$A$1:$D$1</definedName>
+    <definedName hidden="1" localSheetId="21" name="_xlnm._FilterDatabase">'!!References'!$A$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
@@ -742,14 +742,14 @@
     <xf applyAlignment="1" borderId="7" fillId="0" fontId="22" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="41"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="25" fontId="17" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="25" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="42"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="13" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
@@ -759,7 +759,7 @@
     <xf applyAlignment="1" borderId="7" fillId="0" fontId="26" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="43"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="6" fontId="11" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1150,7 +1150,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -1167,42 +1167,38 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Schema' ObjTablesVersion='0.0.8'</t>
+          <t>!!!ObjTables ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="19" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>!!ObjTables Type='Schema' ObjTablesVersion='0.0.8'</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="19" t="inlineStr">
         <is>
           <t>!Table</t>
         </is>
       </c>
-      <c r="B2" s="19" t="inlineStr">
+      <c r="B3" s="19" t="inlineStr">
         <is>
           <t>!Description</t>
         </is>
       </c>
-      <c r="C2" s="19" t="inlineStr">
+      <c r="C3" s="19" t="inlineStr">
         <is>
           <t>!Number of objects</t>
         </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="20" t="inlineStr">
-        <is>
-          <t>Model</t>
-        </is>
-      </c>
-      <c r="B3" s="20" t="n"/>
-      <c r="C3" s="20" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="20" t="inlineStr">
         <is>
-          <t>Taxon</t>
+          <t>Model</t>
         </is>
       </c>
       <c r="B4" s="20" t="n"/>
@@ -1213,7 +1209,7 @@
     <row r="5">
       <c r="A5" s="20" t="inlineStr">
         <is>
-          <t>Environment</t>
+          <t>Taxon</t>
         </is>
       </c>
       <c r="B5" s="20" t="n"/>
@@ -1224,220 +1220,231 @@
     <row r="6">
       <c r="A6" s="20" t="inlineStr">
         <is>
-          <t>Submodels</t>
+          <t>Environment</t>
         </is>
       </c>
       <c r="B6" s="20" t="n"/>
       <c r="C6" s="20" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="20" t="inlineStr">
         <is>
-          <t>Compartments</t>
+          <t>Submodels</t>
         </is>
       </c>
       <c r="B7" s="20" t="n"/>
       <c r="C7" s="20" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="20" t="inlineStr">
         <is>
-          <t>Species types</t>
+          <t>Compartments</t>
         </is>
       </c>
       <c r="B8" s="20" t="n"/>
       <c r="C8" s="20" t="n">
-        <v>143</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="20" t="inlineStr">
         <is>
-          <t>Species</t>
+          <t>Species types</t>
         </is>
       </c>
       <c r="B9" s="20" t="n"/>
       <c r="C9" s="20" t="n">
-        <v>175</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="20" t="inlineStr">
         <is>
-          <t>Initial species concentrations</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B10" s="20" t="n"/>
       <c r="C10" s="20" t="n">
-        <v>125</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="20" t="inlineStr">
         <is>
-          <t>Observables</t>
+          <t>Initial species concentrations</t>
         </is>
       </c>
       <c r="B11" s="20" t="n"/>
       <c r="C11" s="20" t="n">
-        <v>4</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="20" t="inlineStr">
         <is>
-          <t>Functions</t>
+          <t>Observables</t>
         </is>
       </c>
       <c r="B12" s="20" t="n"/>
       <c r="C12" s="20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="20" t="inlineStr">
         <is>
-          <t>Reactions</t>
+          <t>Functions</t>
         </is>
       </c>
       <c r="B13" s="20" t="n"/>
       <c r="C13" s="20" t="n">
-        <v>175</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="20" t="inlineStr">
         <is>
-          <t>Rate laws</t>
+          <t>Reactions</t>
         </is>
       </c>
       <c r="B14" s="20" t="n"/>
       <c r="C14" s="20" t="n">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="20" t="inlineStr">
         <is>
-          <t>dFBA objectives</t>
+          <t>Rate laws</t>
         </is>
       </c>
       <c r="B15" s="20" t="n"/>
       <c r="C15" s="20" t="n">
-        <v>1</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="20" t="inlineStr">
         <is>
-          <t>dFBA objective reactions</t>
+          <t>dFBA objectives</t>
         </is>
       </c>
       <c r="B16" s="20" t="n"/>
       <c r="C16" s="20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="20" t="inlineStr">
         <is>
-          <t>dFBA objective species</t>
+          <t>dFBA objective reactions</t>
         </is>
       </c>
       <c r="B17" s="20" t="n"/>
       <c r="C17" s="20" t="n">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="20" t="inlineStr">
         <is>
-          <t>Parameters</t>
+          <t>dFBA objective species</t>
         </is>
       </c>
       <c r="B18" s="20" t="n"/>
       <c r="C18" s="20" t="n">
-        <v>95</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="20" t="inlineStr">
         <is>
-          <t>Stop conditions</t>
+          <t>Parameters</t>
         </is>
       </c>
       <c r="B19" s="20" t="n"/>
       <c r="C19" s="20" t="n">
-        <v>2</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="20" t="inlineStr">
         <is>
-          <t>Observations</t>
+          <t>Stop conditions</t>
         </is>
       </c>
       <c r="B20" s="20" t="n"/>
       <c r="C20" s="20" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="20" t="inlineStr">
         <is>
-          <t>Observation sets</t>
+          <t>Observations</t>
         </is>
       </c>
       <c r="B21" s="20" t="n"/>
       <c r="C21" s="20" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="20" t="inlineStr">
         <is>
-          <t>Conclusions</t>
+          <t>Observation sets</t>
         </is>
       </c>
       <c r="B22" s="20" t="n"/>
       <c r="C22" s="20" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="20" t="inlineStr">
         <is>
-          <t>References</t>
+          <t>Conclusions</t>
         </is>
       </c>
       <c r="B23" s="20" t="n"/>
       <c r="C23" s="20" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="20" t="inlineStr">
         <is>
-          <t>Authors</t>
+          <t>References</t>
         </is>
       </c>
       <c r="B24" s="20" t="n"/>
       <c r="C24" s="20" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="20" t="inlineStr">
         <is>
-          <t>Changes</t>
+          <t>Authors</t>
         </is>
       </c>
       <c r="B25" s="20" t="n"/>
       <c r="C25" s="20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="20" t="inlineStr">
+        <is>
+          <t>Changes</t>
+        </is>
+      </c>
+      <c r="B26" s="20" t="n"/>
+      <c r="C26" s="20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1496,7 +1503,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Observable' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Observable' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1588,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Function' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Function' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -1662,7 +1669,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:XFD7"/>
+  <dimension ref="A1:AMM7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomRight" state="frozen" topLeftCell="B3" xSplit="1" ySplit="2"/>
@@ -1686,7 +1693,7 @@
     <row customHeight="1" ht="13.5" r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Reaction' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Reaction' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -3969,7 +3976,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='RateLaw' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='RateLaw' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -4178,7 +4185,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:XFD2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
@@ -4196,7 +4203,7 @@
     <row customHeight="1" ht="15.1" r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='DfbaObjective' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='DfbaObjective' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -4292,7 +4299,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='DfbaObjReaction' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='DfbaObjReaction' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -4380,7 +4387,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='DfbaObjSpecies' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='DfbaObjSpecies' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -4478,7 +4485,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Parameter' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Parameter' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -4742,7 +4749,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='StopCondition' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='StopCondition' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -4806,7 +4813,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:XFC3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="2"/>
@@ -4824,7 +4831,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Observation' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Observation' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -5003,7 +5010,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Model' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Model' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -5164,7 +5171,7 @@
     <row customHeight="1" ht="15.1" r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='ObservationSet' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='ObservationSet' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -5248,7 +5255,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Conclusion' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Conclusion' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -5405,7 +5412,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Reference' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Reference' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -5532,7 +5539,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Author' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Author' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -5627,7 +5634,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Change' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Change' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -5747,7 +5754,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Taxon' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Taxon' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -5844,7 +5851,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Environment' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Environment' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -5942,7 +5949,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Submodel' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Submodel' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -6069,7 +6076,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:XFD4"/>
+  <dimension ref="A1:AMR4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="2"/>
@@ -6088,7 +6095,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Compartment' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Compartment' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -8355,7 +8362,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='SpeciesType' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='SpeciesType' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -8550,7 +8557,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='Species' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='Species' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
@@ -8711,7 +8718,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables TableType='Data' ModelId='DistributionInitConcentration' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables Type='Data' Id='DistributionInitConcentration' ObjTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
clean up models, docstring, todo
</commit_message>
<xml_diff>
--- a/examples/transcription_translation_hybrid_model/model.xlsx
+++ b/examples/transcription_translation_hybrid_model/model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28700" windowHeight="13960" tabRatio="993"/>
+    <workbookView xWindow="-24940" yWindow="1800" windowWidth="24940" windowHeight="15700" tabRatio="993" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'!!dFBA objective reactions'!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'!!dFBA objective species'!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'!!Functions'!$A$1:$D$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'[16]!!Initial species concentration'!$A$1:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'[1]!!Initial species concentration'!$A$1:$E$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'!!Model'!$A$1:$B$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'!!Observables'!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'!!Parameters'!$A$1:$H$10</definedName>
@@ -72,69 +72,68 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'!!Stop conditions'!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'!!Submodels'!$A$1:$G$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'!!Taxon'!$A$1:$A$6</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="5">[4]Compartments!$A$2:$H$2</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="14">'[11]dFBA objective reactions'!$A$1:$E$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="15">'[12]dFBA objective species'!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="10">[8]Functions!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="5">[2]Compartments!$A$2:$H$2</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="14">'[3]dFBA objective reactions'!$A$1:$E$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="15">'[4]dFBA objective species'!$A$1:$G$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="10">[5]Functions!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="8">'[6]Initial species concentrations'!$A$1:$E$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="1">[1]Model!$A$1:$B$7</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="9">[7]Observables!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="16">[13]Parameters!$A$1:$H$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="1">[7]Model!$A$1:$B$7</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="9">[8]Observables!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="16">[9]Parameters!$A$1:$H$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="12">'[10]Rate laws'!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="11">[9]Reactions!$A$2:$J$2</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="21">[15]References!$A$1:$Q$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="6">'[5]Species types'!$A$2:$K$2</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="11">[11]Reactions!$A$2:$J$2</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="21">[12]References!$A$1:$Q$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="6">'[13]Species types'!$A$2:$K$2</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="17">'[14]Stop conditions'!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="4">[3]Submodels!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="2">[2]Taxon!$A$1:$A$5</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="5">[4]Compartments!$A$2:$H$2</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="14">'[11]dFBA objective reactions'!$A$1:$E$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="15">'[12]dFBA objective species'!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="10">[8]Functions!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="4">[15]Submodels!$A$1:$G$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="2">[16]Taxon!$A$1:$A$5</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="5">[2]Compartments!$A$2:$H$2</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="14">'[3]dFBA objective reactions'!$A$1:$E$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="15">'[4]dFBA objective species'!$A$1:$G$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="10">[5]Functions!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="8">'[6]Initial species concentrations'!$A$1:$E$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="1">[1]Model!$A$1:$B$7</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="9">[7]Observables!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="16">[13]Parameters!$A$1:$H$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="1">[7]Model!$A$1:$B$7</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="9">[8]Observables!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="16">[9]Parameters!$A$1:$H$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="12">'[10]Rate laws'!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="11">[9]Reactions!$A$2:$J$2</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="21">[15]References!$A$1:$Q$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$2</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="11">[11]Reactions!$A$2:$J$2</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="21">[12]References!$A$1:$Q$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="6">'[13]Species types'!$A$2:$K$2</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="17">'[14]Stop conditions'!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="4">[3]Submodels!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="2">[2]Taxon!$A$1:$A$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">[4]Compartments!$A$2:$H$2</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="14">'[11]dFBA objective reactions'!$A$1:$E$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="15">'[12]dFBA objective species'!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="10">[8]Functions!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="4">[15]Submodels!$A$1:$G$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="2">[16]Taxon!$A$1:$A$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">[2]Compartments!$A$2:$H$2</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="14">'[3]dFBA objective reactions'!$A$1:$E$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="15">'[4]dFBA objective species'!$A$1:$G$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="10">[5]Functions!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="8">'[6]Initial species concentrations'!$A$1:$E$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="1">[1]Model!$A$1:$B$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="9">[7]Observables!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="16">[13]Parameters!$A$1:$H$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="1">[7]Model!$A$1:$B$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="9">[8]Observables!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="16">[9]Parameters!$A$1:$H$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="12">'[10]Rate laws'!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="11">[9]Reactions!$A$2:$J$2</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="21">[15]References!$A$1:$Q$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$2</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="11">[11]Reactions!$A$2:$J$2</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="21">[12]References!$A$1:$Q$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'[13]Species types'!$A$2:$K$2</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="17">'[14]Stop conditions'!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="4">[3]Submodels!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="2">[2]Taxon!$A$1:$A$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">[4]Compartments!$A$2:$H$2</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="14">'[11]dFBA objective reactions'!$A$1:$E$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="15">'[12]dFBA objective species'!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="10">[8]Functions!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="4">[15]Submodels!$A$1:$G$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="2">[16]Taxon!$A$1:$A$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">[2]Compartments!$A$2:$H$2</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="14">'[3]dFBA objective reactions'!$A$1:$E$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="15">'[4]dFBA objective species'!$A$1:$G$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="10">[5]Functions!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="8">'[6]Initial species concentrations'!$A$1:$E$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="1">[1]Model!$A$1:$B$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="9">[7]Observables!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="16">[13]Parameters!$A$1:$H$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="1">[7]Model!$A$1:$B$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="9">[8]Observables!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="16">[9]Parameters!$A$1:$H$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="12">'[10]Rate laws'!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="11">[9]Reactions!$A$2:$J$2</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="21">[15]References!$A$1:$Q$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$2</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="11">[11]Reactions!$A$2:$J$2</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="21">[12]References!$A$1:$Q$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'[13]Species types'!$A$2:$K$2</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="17">'[14]Stop conditions'!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="4">[3]Submodels!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="2">[2]Taxon!$A$1:$A$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="4">[15]Submodels!$A$1:$G$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="2">[16]Taxon!$A$1:$A$5</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1018,7 +1017,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Model"/>
+      <sheetName val="!!Initial species concentration"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1044,7 +1043,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="dFBA objective reactions"/>
+      <sheetName val="Reactions"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1057,7 +1056,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="dFBA objective species"/>
+      <sheetName val="References"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1070,7 +1069,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Parameters"/>
+      <sheetName val="Species types"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1096,7 +1095,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="References"/>
+      <sheetName val="Submodels"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1109,7 +1108,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="!!Initial species concentration"/>
+      <sheetName val="Taxon"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1122,7 +1121,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Taxon"/>
+      <sheetName val="Compartments"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1135,7 +1134,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Submodels"/>
+      <sheetName val="dFBA objective reactions"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1148,7 +1147,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Compartments"/>
+      <sheetName val="dFBA objective species"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1161,7 +1160,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Species types"/>
+      <sheetName val="Functions"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1187,7 +1186,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Observables"/>
+      <sheetName val="Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1200,7 +1199,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Functions"/>
+      <sheetName val="Observables"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1213,7 +1212,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Reactions"/>
+      <sheetName val="Parameters"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1482,7 +1481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
@@ -1756,11 +1755,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection activeCell="A6" sqref="A6"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1815,11 +1815,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection activeCell="A6" sqref="A6"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1887,11 +1888,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection activeCell="A6" sqref="A6"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1899,8 +1901,9 @@
     <col min="1" max="1" width="16" style="3" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="3" customWidth="1"/>
     <col min="7" max="1027" width="8.5" style="3" customWidth="1"/>
     <col min="1028" max="1028" width="9" style="3" customWidth="1"/>
     <col min="1029" max="16384" width="9" style="3"/>
@@ -4093,11 +4096,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="A6" sqref="A6"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4106,7 +4110,7 @@
     <col min="2" max="2" width="8.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" style="3" customWidth="1"/>
     <col min="4" max="5" width="12.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="50.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="12.6640625" style="3" customWidth="1"/>
     <col min="11" max="11" width="8.5" style="3" customWidth="1"/>
     <col min="12" max="13" width="12.6640625" style="3" customWidth="1"/>
@@ -4120,7 +4124,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>29</v>
       </c>
@@ -5491,18 +5495,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" style="3" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" style="3" customWidth="1"/>
-    <col min="3" max="1026" width="8.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="1026" width="8.5" style="3" customWidth="1"/>
     <col min="1027" max="1027" width="9" style="3" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="3"/>
   </cols>
@@ -5593,11 +5598,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMR4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection activeCell="A6" sqref="A6"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7788,11 +7794,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection activeCell="A6" sqref="A6"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7933,11 +7940,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection activeCell="A6" sqref="A6"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8041,11 +8049,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="A6" sqref="A6"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>